<commit_message>
feat(inventory): collect items from the world to the inventory (#1)
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -34,16 +34,16 @@
     <t xml:space="preserve">GAME_NAME</t>
   </si>
   <si>
-    <t xml:space="preserve">Godot 4.3</t>
+    <t xml:space="preserve">Kyukodo</t>
   </si>
   <si>
     <t xml:space="preserve">GAME_TAGLINE</t>
   </si>
   <si>
-    <t xml:space="preserve">2D Template</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Template 2D</t>
+    <t xml:space="preserve">Setup the planet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Préparation de planète</t>
   </si>
   <si>
     <t xml:space="preserve">MAIN_START_BUTTON</t>
@@ -143,6 +143,24 @@
   </si>
   <si>
     <t xml:space="preserve">RETOUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITEM_USE_BUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utiliser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITEM_DROP_BUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeter</t>
   </si>
 </sst>
 </file>
@@ -224,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -235,6 +253,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -360,10 +382,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -401,7 +423,7 @@
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -524,6 +546,28 @@
       </c>
       <c r="C14" s="1" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(item-resource): translate collecting hint
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t xml:space="preserve">Jeter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESOURCE_COLLECT_WITH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collect with</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Récolter avec</t>
   </si>
 </sst>
 </file>
@@ -382,10 +391,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -570,6 +579,17 @@
         <v>46</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat(item-resource): implement Item resources (stone + gold) (#2)
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t xml:space="preserve">Jeter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESOURCE_COLLECT_WITH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collect with</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Récolter avec</t>
   </si>
 </sst>
 </file>
@@ -382,10 +391,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -570,6 +579,17 @@
         <v>46</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat(camp): save/restore player when leaving camp
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t xml:space="preserve">fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMP_RETURN_TO_PLANETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rerturn to planet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retour à la planète</t>
   </si>
   <si>
     <t xml:space="preserve">GAME_NAME</t>
@@ -391,10 +400,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -422,17 +431,17 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -443,7 +452,7 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -589,6 +598,20 @@
       <c r="C17" s="1" t="s">
         <v>49</v>
       </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat(camp): implement entering and exiting the camp (#3)
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t xml:space="preserve">fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMP_RETURN_TO_PLANETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return to planet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retour à la planète</t>
   </si>
   <si>
     <t xml:space="preserve">GAME_NAME</t>
@@ -391,10 +400,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -422,17 +431,17 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -443,7 +452,7 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -588,6 +597,17 @@
       </c>
       <c r="C17" s="1" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(house): implement upgrade panel
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -179,6 +179,36 @@
   </si>
   <si>
     <t xml:space="preserve">Récolter avec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPGRADE_TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPGRADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMÉLIORER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPGRADE_STONE_LABEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pierre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPGRADE_GOLD_LABEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPGRADE_BUTTON</t>
   </si>
 </sst>
 </file>
@@ -400,10 +430,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -610,6 +640,50 @@
         <v>52</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat(house): implement houses (#4)
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -179,6 +179,36 @@
   </si>
   <si>
     <t xml:space="preserve">Récolter avec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPGRADE_TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPGRADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMÉLIORER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPGRADE_STONE_LABEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pierre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPGRADE_GOLD_LABEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPGRADE_BUTTON</t>
   </si>
 </sst>
 </file>
@@ -400,10 +430,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -610,6 +640,50 @@
         <v>52</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat(objective): translate button to finish the current objective
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -209,6 +209,60 @@
   </si>
   <si>
     <t xml:space="preserve">UPGRADE_BUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBJECTIVE_TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ongoing objective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objectif en cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBJECTIVE_FINISH_BUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBJECTIVE_MAKE_SOME_STEPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Before all, let’s walk some steps.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avant toute chose, dégourdissez-vous les pattes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBJECTIVE_COLLECT_FOR_TENTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To setup your camp : collect 10 stone units.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afin de construire construire votre camp : récoltez 10 unités de pierre.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBJECTIVE_BUILD_FIRST_TENTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start setuping your camp, build first tents.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Débutez l’installation de votre campement, construisez les premières tentes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBJECTIVE_THE_END</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congratulations, you’ve finished the objectives.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Félicitation, vous avez fini les objectifs.</t>
   </si>
 </sst>
 </file>
@@ -430,16 +484,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="62.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -682,6 +737,72 @@
       </c>
       <c r="C22" s="1" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(pause): implement the pause menu
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -263,6 +263,24 @@
   </si>
   <si>
     <t xml:space="preserve">Félicitation, vous avez fini les objectifs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAUSE_TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAUSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAUSE_RESUME_BUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reprendre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAUSE_QUIT_BUTTON</t>
   </si>
 </sst>
 </file>
@@ -484,10 +502,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -805,6 +823,39 @@
         <v>80</v>
       </c>
     </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat(camp): add camp title
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="90">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -40,6 +40,15 @@
     <t xml:space="preserve">Retour à la planète</t>
   </si>
   <si>
+    <t xml:space="preserve">CAMP_TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to the camp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bienvenu au campement</t>
+  </si>
+  <si>
     <t xml:space="preserve">GAME_NAME</t>
   </si>
   <si>
@@ -244,7 +253,7 @@
     <t xml:space="preserve">To setup your camp : collect 10 stone units.</t>
   </si>
   <si>
-    <t xml:space="preserve">Afin de construire construire votre camp : récoltez 10 unités de pierre.</t>
+    <t xml:space="preserve">Afin de construire construire votre campement : récoltez 10 unités de pierre.</t>
   </si>
   <si>
     <t xml:space="preserve">OBJECTIVE_BUILD_FIRST_TENTS</t>
@@ -502,10 +511,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -545,17 +556,17 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -566,7 +577,7 @@
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -751,21 +762,21 @@
         <v>62</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,15 +842,15 @@
         <v>82</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>85</v>
@@ -850,10 +861,21 @@
         <v>86</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>25</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(objective): add secret objective to finish the camp
</commit_message>
<xml_diff>
--- a/resources/localization/MenuTranslations.xlsx
+++ b/resources/localization/MenuTranslations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -272,6 +272,15 @@
   </si>
   <si>
     <t xml:space="preserve">Félicitation, vous avez fini les objectifs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBJECTIVE_GAME_FINISHED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You stayed strong! Congratulations, you finished the camp!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vous n’avez rien lâché ! Félicitions, vous avez fini votre campement !</t>
   </si>
   <si>
     <t xml:space="preserve">PAUSE_TITLE</t>
@@ -511,18 +520,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="bottomLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="50.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="62.2"/>
   </cols>
   <sheetData>
@@ -853,15 +862,15 @@
         <v>85</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>88</v>
@@ -872,9 +881,20 @@
         <v>89</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>